<commit_message>
Adding work with furloughs: adding, editing, deleting, and printing lists
</commit_message>
<xml_diff>
--- a/wwwroot/Templates/Dismissals/returning_recruits.xlsx
+++ b/wwwroot/Templates/Dismissals/returning_recruits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SPRT\wwwroot\Templates\Dismissals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NewSprt\wwwroot\Templates\Dismissals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48162F99-9F2B-4867-BE32-C941451AE2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321DECA-3ED1-4F03-B4DC-E9485A303A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,10 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Dismissals">Лист1!$A$4:$G$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$B$1:$G$9</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -29,46 +33,45 @@
     <t>Дата  рождения</t>
   </si>
   <si>
-    <t>#NUM</t>
-  </si>
-  <si>
-    <t>#BIRTHDATE</t>
-  </si>
-  <si>
-    <t>#COMISSARIAT</t>
-  </si>
-  <si>
-    <t>#FIO</t>
-  </si>
-  <si>
     <t>ФИО</t>
   </si>
   <si>
+    <t>Дата убытия</t>
+  </si>
+  <si>
+    <t>Примечания</t>
+  </si>
+  <si>
+    <t>Военный комиссариат</t>
+  </si>
+  <si>
+    <t>{{item.Index}}</t>
+  </si>
+  <si>
+    <t>{{item.FullName}}</t>
+  </si>
+  <si>
+    <t>{{item.BirthDate}}</t>
+  </si>
+  <si>
+    <t>{{item.MilitaryComissariat}}</t>
+  </si>
+  <si>
+    <t>{{item.SendDismissalDate}}</t>
+  </si>
+  <si>
+    <t>{{item.Notice}}</t>
+  </si>
+  <si>
+    <t>Начальник отдела (подготовки и призыва граждан на военную службу)</t>
+  </si>
+  <si>
+    <t>полковник                                                                                       И.Каримов</t>
+  </si>
+  <si>
     <t>Список
-граждан, призванных на военную службу Военным комиссариатом Республики Татарстан
-и находящихся в увольнении до #DATE_TO</t>
-  </si>
-  <si>
-    <t>Дата убытия</t>
-  </si>
-  <si>
-    <t>Примечания</t>
-  </si>
-  <si>
-    <t>#NOTICE</t>
-  </si>
-  <si>
-    <t>#DATE_FROM</t>
-  </si>
-  <si>
-    <t>Военный комиссариат</t>
-  </si>
-  <si>
-    <t>Начальник отдела 
-(подготовки и призыва граждан на военную службу)</t>
-  </si>
-  <si>
-    <t>полковник                                                                                    И.Каримов</t>
+граждан, призванных на военную службу Военным комиссариатом Республики Татарстан 
+и находящихся в увольнении до {{ReturnDate}}</t>
   </si>
 </sst>
 </file>
@@ -142,30 +145,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,103 +517,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="B1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="0.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="2:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="G7" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="B1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>